<commit_message>
Clean up code and run outputs
</commit_message>
<xml_diff>
--- a/model/Inputs/model_inputs_inelas.xlsx
+++ b/model/Inputs/model_inputs_inelas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEF60969-7FA7-4919-A048-32EF02B4D913}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{485B9A51-2018-4F80-A3E4-ED40EE7F4766}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -209,7 +209,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
@@ -269,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -286,6 +287,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,10 +1053,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1062,13 +1064,14 @@
     <col min="1" max="1" width="27.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>1.4000710227272728E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1156,6 +1159,84 @@
       <c r="G4" s="7">
         <v>5.9999999999999995E-4</v>
       </c>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K29" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1376,7 +1457,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1422,7 +1503,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Y3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2600,6 +2681,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D835CF4C7D56B243BA013D4D2E10914B" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e645ef68b9493f2ee8bae9e534bc24f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6d4e152b-60f6-4719-8921-68b5b8011cde" xmlns:ns4="28683373-984a-4841-9f0e-018f3f7bab1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a06da6e71fc3d3bdf7cbe176c2a8afa1" ns3:_="" ns4:_="">
     <xsd:import namespace="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
@@ -2852,7 +2941,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2861,15 +2950,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCE4FBA5-6C26-4B97-9218-92B658F853C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2888,27 +2986,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Change input of interest and DG annual capacity
</commit_message>
<xml_diff>
--- a/model/Inputs/model_inputs_inelas.xlsx
+++ b/model/Inputs/model_inputs_inelas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/Model-1/model/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{485B9A51-2018-4F80-A3E4-ED40EE7F4766}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="6_{7DA8CDEE-914B-4384-BE83-347F050180D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46F652FA-F727-4064-856E-B698EF06B5F6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>min SoC</t>
   </si>
   <si>
-    <t>Interest rate</t>
-  </si>
-  <si>
     <t>Battery Eff</t>
   </si>
   <si>
@@ -203,6 +200,9 @@
   </si>
   <si>
     <t>Allow PV</t>
+  </si>
+  <si>
+    <t>DG annual capacity</t>
   </si>
 </sst>
 </file>
@@ -521,10 +521,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,15 +843,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.90625" customWidth="1"/>
     <col min="8" max="8" width="11.08984375" bestFit="1" customWidth="1"/>
@@ -867,28 +863,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>49</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -896,7 +892,7 @@
         <v>0.02</v>
       </c>
       <c r="B2">
-        <v>0.11</v>
+        <v>0.8</v>
       </c>
       <c r="C2">
         <v>0.99</v>
@@ -1017,15 +1013,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>635</v>
@@ -1036,7 +1032,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1055,7 +1051,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1073,27 +1069,27 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>400</v>
@@ -1116,7 +1112,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1139,7 +1135,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1260,12 +1256,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0.80323299888517286</v>
@@ -1273,7 +1269,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0.7998018797075267</v>
@@ -1281,7 +1277,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0.79636610600256064</v>
@@ -1289,7 +1285,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>0.79292564496168683</v>
@@ -1297,7 +1293,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>0.78948046335616628</v>
@@ -1305,7 +1301,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>0.78603052752928926</v>
@@ -1313,7 +1309,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>0.78257580338835164</v>
@@ -1321,7 +1317,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>0.77911625639644011</v>
@@ -1329,7 +1325,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>0.77565185156400585</v>
@@ -1337,7 +1333,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>0.77218255344024267</v>
@@ -1345,7 +1341,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>0.76870832610423512</v>
@@ -1353,7 +1349,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>0.76522913315588315</v>
@@ -1361,7 +1357,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>0.76174493770661011</v>
@@ -1369,7 +1365,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>0.75825570236981887</v>
@@ -1377,7 +1373,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>0.75476138925110314</v>
@@ -1408,12 +1404,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <f>(-0.2129*(0.3^3+0^3) +0.6056*(0.3^2+0^2) - 0.5538*(0.3+0) + 0.4067*2)/2</f>
@@ -1425,7 +1421,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <f>(-0.2129*(0.6^3+0.3^3) +0.6056*(0.6^2+0.3^2) - 0.5538*(0.6+0.3) + 0.4067*2)/2</f>
@@ -1437,7 +1433,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <f>(-0.2129*(1^3+0.6^3) +0.6056*(1^2+0.6^2) - 0.5538*(1+0.6) + 0.4067*2)/2</f>
@@ -1465,12 +1461,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>199</v>
@@ -1478,7 +1474,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>106</v>
@@ -1486,7 +1482,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>60</v>
@@ -1588,7 +1584,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1665,7 +1661,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1742,7 +1738,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1912,7 +1908,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4">
         <v>0.52236078409734032</v>
@@ -1989,7 +1985,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4">
         <v>0.4532206627457997</v>
@@ -2066,7 +2062,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4">
         <v>0.38408054139425912</v>
@@ -2351,7 +2347,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4">
         <v>0.3415913978494623</v>
@@ -2428,7 +2424,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4">
         <v>0.21991235409714491</v>
@@ -2505,7 +2501,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4">
         <v>9.8233310344827587E-2</v>
@@ -2681,11 +2677,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2942,27 +2939,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d4e152b-60f6-4719-8921-68b5b8011cde" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2987,9 +2974,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCE34160-36D4-4F46-97A9-A281FB44CDD4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95B8A76-94F3-412F-9855-4B93BB4C4C10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="28683373-984a-4841-9f0e-018f3f7bab1f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6d4e152b-60f6-4719-8921-68b5b8011cde"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>